<commit_message>
21/06/19: simplification, cleaning du code, fragmentation en petites fonctions
</commit_message>
<xml_diff>
--- a/INPUT/DATA_IN.xlsx
+++ b/INPUT/DATA_IN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jim/Documents/Work/Facette_36Cl/Facet_36Cl_CREp/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{174EBAC8-2078-AC4B-BF58-6CD851A8D038}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6DB3D15-CFC7-F34A-96FB-219B7706D86F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-36920" yWindow="-3840" windowWidth="35720" windowHeight="9600" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,13 +16,18 @@
     <sheet name="Sample" sheetId="1" r:id="rId1"/>
     <sheet name="Parameters" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179021" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -5305,7 +5310,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5882,7 +5887,7 @@
         <v>117</v>
       </c>
       <c r="B36" s="16">
-        <v>300000</v>
+        <v>2000</v>
       </c>
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="s">
@@ -5991,7 +5996,7 @@
         <v>128</v>
       </c>
       <c r="B43" s="16">
-        <v>2.8</v>
+        <v>2</v>
       </c>
       <c r="C43" s="16"/>
       <c r="D43" s="16" t="s">
@@ -6008,7 +6013,7 @@
         <v>130</v>
       </c>
       <c r="B44" s="46">
-        <v>32000</v>
+        <v>20000</v>
       </c>
       <c r="C44" s="16"/>
       <c r="D44" s="16" t="s">

</xml_diff>

<commit_message>
Update readme and fix some bugs. La version multisites est maintenant la version normale
</commit_message>
<xml_diff>
--- a/INPUT/DATA_IN.xlsx
+++ b/INPUT/DATA_IN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jim/Documents/Work/Facette_36Cl/Facet_36Cl_CREp/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217DA6F6-D9F1-544D-91E9-11410F163AB9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E9330E-EF11-5545-B3A4-889B58A1DD6C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24700" yWindow="-5140" windowWidth="25600" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28640" yWindow="-4160" windowWidth="25600" windowHeight="18060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="149">
   <si>
     <t>sample name</t>
   </si>
@@ -369,12 +369,6 @@
     <t xml:space="preserve"> (mm/yr) Inversion maximum slip-rate bound</t>
   </si>
   <si>
-    <t>SR_std</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (mm/yr) Standart deviation for normal distribution of the proposal function</t>
-  </si>
-  <si>
     <t>T_min</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
   </si>
   <si>
     <t xml:space="preserve">(yr) Inversion maximum post-glacial age bound </t>
-  </si>
-  <si>
-    <t>T_std</t>
   </si>
   <si>
     <t>n_walker</t>
@@ -574,7 +565,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -608,6 +599,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -651,7 +648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -763,12 +760,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -858,12 +849,28 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1179,10 +1186,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C226010C-3229-414E-B3FA-2CD5555C7F40}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1193,13 +1200,13 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>150</v>
-      </c>
-      <c r="B1" s="78">
-        <v>2</v>
-      </c>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
+        <v>147</v>
+      </c>
+      <c r="B1" s="76">
+        <v>4</v>
+      </c>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
       <c r="E1" s="23"/>
       <c r="F1" s="23"/>
       <c r="G1" s="23"/>
@@ -1208,19 +1215,19 @@
     </row>
     <row r="2" spans="1:9" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="47" t="s">
+        <v>141</v>
+      </c>
+      <c r="B2" s="77" t="s">
         <v>66</v>
       </c>
-      <c r="C2" s="47" t="s">
-        <v>127</v>
-      </c>
-      <c r="D2" s="47" t="s">
-        <v>128</v>
-      </c>
-      <c r="E2" s="47" t="s">
-        <v>129</v>
+      <c r="C2" s="77" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="77" t="s">
+        <v>125</v>
+      </c>
+      <c r="E2" s="77" t="s">
+        <v>126</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="17"/>
@@ -1231,17 +1238,17 @@
       <c r="A3" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="78">
         <v>1275</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="78">
         <f>1265+15</f>
         <v>1280</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="78">
         <v>815</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="78">
         <f>635+8</f>
         <v>643</v>
       </c>
@@ -1254,16 +1261,16 @@
       <c r="A4" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="78">
         <v>30</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4" s="78">
         <v>25</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="78">
         <v>25</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="78">
         <v>25</v>
       </c>
       <c r="F4" s="17"/>
@@ -1275,16 +1282,16 @@
       <c r="A5" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="78">
         <v>45</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="78">
         <v>40</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="78">
         <v>55</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="78">
         <v>65</v>
       </c>
       <c r="F5" s="17"/>
@@ -1296,16 +1303,16 @@
       <c r="A6" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6" s="78">
         <v>35</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="78">
         <v>30</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="78">
         <v>30</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="78">
         <v>35</v>
       </c>
       <c r="F6" s="17"/>
@@ -1317,16 +1324,16 @@
       <c r="A7" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7" s="78">
         <v>1.6</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="78">
         <v>1.5</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="78">
         <v>1.5</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="78">
         <v>1.5</v>
       </c>
       <c r="F7" s="17"/>
@@ -1362,7 +1369,7 @@
       <c r="A10" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="79">
         <v>160</v>
       </c>
       <c r="C10" s="17"/>
@@ -1379,7 +1386,7 @@
       <c r="A11" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="79">
         <v>208</v>
       </c>
       <c r="C11" s="17"/>
@@ -1396,7 +1403,7 @@
       <c r="A12" s="17" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="79">
         <v>1510</v>
       </c>
       <c r="C12" s="17"/>
@@ -1413,7 +1420,7 @@
       <c r="A13" s="17" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="79">
         <v>190</v>
       </c>
       <c r="C13" s="17"/>
@@ -1430,7 +1437,7 @@
       <c r="A14" s="40" t="s">
         <v>76</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="80">
         <v>42.2</v>
       </c>
       <c r="C14" s="40"/>
@@ -1447,7 +1454,7 @@
       <c r="A15" s="41" t="s">
         <v>78</v>
       </c>
-      <c r="B15" s="41">
+      <c r="B15" s="81">
         <v>148.1</v>
       </c>
       <c r="C15" s="41"/>
@@ -1464,7 +1471,7 @@
       <c r="A16" s="41" t="s">
         <v>80</v>
       </c>
-      <c r="B16" s="41">
+      <c r="B16" s="81">
         <v>13</v>
       </c>
       <c r="C16" s="41"/>
@@ -1481,7 +1488,7 @@
       <c r="A17" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="B17" s="42">
+      <c r="B17" s="82">
         <v>1.9</v>
       </c>
       <c r="C17" s="42"/>
@@ -1498,7 +1505,7 @@
       <c r="A18" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="80">
         <v>4.8</v>
       </c>
       <c r="C18" s="40"/>
@@ -1515,7 +1522,7 @@
       <c r="A19" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="B19" s="41">
+      <c r="B19" s="81">
         <v>7.8</v>
       </c>
       <c r="C19" s="41"/>
@@ -1532,7 +1539,7 @@
       <c r="A20" s="41" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="41">
+      <c r="B20" s="81">
         <v>3</v>
       </c>
       <c r="C20" s="41"/>
@@ -1549,7 +1556,7 @@
       <c r="A21" s="41" t="s">
         <v>90</v>
       </c>
-      <c r="B21" s="41">
+      <c r="B21" s="81">
         <v>0.2</v>
       </c>
       <c r="C21" s="41"/>
@@ -1566,7 +1573,7 @@
       <c r="A22" s="40" t="s">
         <v>92</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="80">
         <v>1</v>
       </c>
       <c r="C22" s="40"/>
@@ -1583,7 +1590,7 @@
       <c r="A23" s="41" t="s">
         <v>94</v>
       </c>
-      <c r="B23" s="41">
+      <c r="B23" s="81">
         <v>3</v>
       </c>
       <c r="C23" s="41"/>
@@ -1600,7 +1607,7 @@
       <c r="A24" s="41" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="41">
+      <c r="B24" s="81">
         <v>0</v>
       </c>
       <c r="C24" s="41"/>
@@ -1641,7 +1648,7 @@
       <c r="A27" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B27" s="79">
         <v>300000</v>
       </c>
       <c r="C27" s="17"/>
@@ -1658,7 +1665,7 @@
       <c r="A28" s="40" t="s">
         <v>101</v>
       </c>
-      <c r="B28" s="40">
+      <c r="B28" s="80">
         <v>15000</v>
       </c>
       <c r="C28" s="40"/>
@@ -1675,7 +1682,7 @@
       <c r="A29" s="42" t="s">
         <v>103</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B29" s="83">
         <v>1</v>
       </c>
       <c r="C29" s="42"/>
@@ -1692,7 +1699,7 @@
       <c r="A30" s="40" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="44">
+      <c r="B30" s="84">
         <v>0</v>
       </c>
       <c r="C30" s="40"/>
@@ -1709,7 +1716,7 @@
       <c r="A31" s="41" t="s">
         <v>107</v>
       </c>
-      <c r="B31" s="45">
+      <c r="B31" s="85">
         <v>5</v>
       </c>
       <c r="C31" s="41"/>
@@ -1723,67 +1730,66 @@
       <c r="I31" s="41"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A32" s="41" t="s">
+      <c r="A32" s="40" t="s">
         <v>109</v>
       </c>
-      <c r="B32" s="45">
-        <v>1.5</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41" t="s">
+      <c r="B32" s="80">
+        <v>0</v>
+      </c>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40" t="s">
         <v>110</v>
       </c>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
-      <c r="G32" s="41"/>
-      <c r="H32" s="41"/>
-      <c r="I32" s="41"/>
+      <c r="E32" s="40"/>
+      <c r="F32" s="40"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A33" s="40" t="s">
+      <c r="A33" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="B33" s="40">
-        <f>12000</f>
-        <v>12000</v>
-      </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40" t="s">
+      <c r="B33" s="79">
+        <v>30000</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="E33" s="40"/>
-      <c r="F33" s="40"/>
-      <c r="G33" s="40"/>
-      <c r="H33" s="40"/>
-      <c r="I33" s="40"/>
+      <c r="E33" s="17"/>
+      <c r="F33" s="17"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="17"/>
+      <c r="I33" s="17"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="40" t="s">
         <v>113</v>
       </c>
-      <c r="B34" s="17">
-        <v>18000</v>
-      </c>
-      <c r="C34" s="17"/>
-      <c r="D34" s="17" t="s">
+      <c r="B34" s="80">
+        <v>10</v>
+      </c>
+      <c r="C34" s="40"/>
+      <c r="D34" s="40" t="s">
         <v>114</v>
       </c>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
+      <c r="E34" s="40"/>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="17" t="s">
         <v>115</v>
       </c>
-      <c r="B35" s="17">
-        <v>2000</v>
+      <c r="B35" s="79">
+        <v>3000</v>
       </c>
       <c r="C35" s="17"/>
-      <c r="D35" s="41" t="s">
-        <v>110</v>
+      <c r="D35" s="17" t="s">
+        <v>116</v>
       </c>
       <c r="E35" s="17"/>
       <c r="F35" s="17"/>
@@ -1792,32 +1798,32 @@
       <c r="I35" s="17"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A36" s="40" t="s">
-        <v>116</v>
-      </c>
-      <c r="B36" s="40">
-        <v>10</v>
-      </c>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40" t="s">
+      <c r="A36" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="E36" s="40"/>
-      <c r="F36" s="40"/>
-      <c r="G36" s="40"/>
-      <c r="H36" s="40"/>
-      <c r="I36" s="40"/>
+      <c r="B36" s="86">
+        <v>1</v>
+      </c>
+      <c r="C36" s="17"/>
+      <c r="D36" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="B37" s="17">
-        <v>1500</v>
+        <v>119</v>
+      </c>
+      <c r="B37" s="86">
+        <v>0.2</v>
       </c>
       <c r="C37" s="17"/>
       <c r="D37" s="17" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E37" s="17"/>
       <c r="F37" s="17"/>
@@ -1827,14 +1833,14 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="B38" s="46">
-        <v>1</v>
+        <v>121</v>
+      </c>
+      <c r="B38" s="86">
+        <v>1000</v>
       </c>
       <c r="C38" s="17"/>
       <c r="D38" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="E38" s="17"/>
       <c r="F38" s="17"/>
@@ -1843,125 +1849,102 @@
       <c r="I38" s="17"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A39" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="B39" s="46">
-        <v>0.2</v>
-      </c>
-      <c r="C39" s="17"/>
-      <c r="D39" s="17" t="s">
+      <c r="A39" s="23"/>
+      <c r="B39" s="23"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23"/>
+      <c r="H39" s="23"/>
+      <c r="I39" s="23"/>
+    </row>
+    <row r="40" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A40" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="E39" s="17"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="17"/>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A40" s="17" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" s="46">
-        <v>1000</v>
-      </c>
-      <c r="C40" s="17"/>
-      <c r="D40" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="E40" s="17"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="17"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="G40" s="23"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A41" s="23"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="23"/>
-      <c r="H41" s="23"/>
-      <c r="I41" s="23"/>
-    </row>
-    <row r="42" spans="1:9" ht="21" x14ac:dyDescent="0.25">
-      <c r="A42" s="15" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="47" t="str">
+      <c r="A41" s="40" t="s">
+        <v>148</v>
+      </c>
+      <c r="B41" s="80">
+        <v>0</v>
+      </c>
+      <c r="C41" s="74"/>
+      <c r="D41" s="74"/>
+      <c r="E41" s="74"/>
+      <c r="F41" s="74"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="74"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="B42" s="86">
+        <v>20000</v>
+      </c>
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+    </row>
+    <row r="43" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A43" s="17"/>
+      <c r="B43" s="43" t="str">
         <f>B2</f>
         <v>MA3</v>
       </c>
-      <c r="C42" s="47" t="str">
+      <c r="C43" s="43" t="str">
         <f>C2</f>
         <v>MA1</v>
       </c>
-      <c r="D42" s="47" t="str">
+      <c r="D43" s="43" t="str">
         <f>D2</f>
         <v>ARC</v>
       </c>
-      <c r="E42" s="47" t="str">
+      <c r="E43" s="43" t="str">
         <f>E2</f>
         <v>BAZ</v>
       </c>
-      <c r="F42" s="17"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="17"/>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A43" s="40" t="s">
-        <v>151</v>
-      </c>
-      <c r="B43" s="40">
-        <v>0</v>
-      </c>
-      <c r="C43" s="79"/>
-      <c r="D43" s="79"/>
-      <c r="E43" s="79"/>
-      <c r="F43" s="79"/>
-      <c r="G43" s="79"/>
-      <c r="H43" s="79"/>
-      <c r="I43" s="79"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="17" t="s">
-        <v>148</v>
-      </c>
-      <c r="B44" s="17">
+        <v>145</v>
+      </c>
+      <c r="B44" s="79">
         <v>2.8</v>
       </c>
-      <c r="C44" s="17">
+      <c r="C44" s="79">
         <v>1.3</v>
       </c>
-      <c r="D44" s="17">
+      <c r="D44" s="79">
         <v>0.5</v>
       </c>
-      <c r="E44" s="17">
+      <c r="E44" s="79">
         <v>0.1</v>
       </c>
       <c r="F44" s="17"/>
       <c r="G44" s="17"/>
       <c r="H44" s="17"/>
       <c r="I44" s="17"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="B45" s="46">
-        <v>20000</v>
-      </c>
-      <c r="C45" s="23"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="23"/>
-      <c r="G45" s="23"/>
-      <c r="H45" s="23"/>
-      <c r="I45" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4264,7 +4247,7 @@
     <col min="24" max="24" width="13.83203125" style="2" customWidth="1"/>
     <col min="25" max="25" width="13.83203125" style="3" customWidth="1"/>
     <col min="26" max="29" width="13.83203125" style="6" customWidth="1"/>
-    <col min="30" max="43" width="13.83203125" style="71" customWidth="1"/>
+    <col min="30" max="43" width="13.83203125" style="67" customWidth="1"/>
     <col min="44" max="46" width="13.83203125" style="10" customWidth="1"/>
     <col min="47" max="47" width="13.83203125" style="8" customWidth="1"/>
     <col min="48" max="49" width="13.83203125" style="10" customWidth="1"/>
@@ -4363,7 +4346,7 @@
       <c r="AD1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="48" t="s">
+      <c r="AE1" s="44" t="s">
         <v>22</v>
       </c>
       <c r="AF1" s="11" t="s">
@@ -4453,26 +4436,26 @@
       <c r="BX1" s="39"/>
       <c r="BY1" s="39"/>
     </row>
-    <row r="2" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
-        <v>130</v>
-      </c>
-      <c r="B2" s="50">
+    <row r="2" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="B2" s="46">
         <v>42.130239330000002</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="47">
         <v>13.413394500000001</v>
       </c>
-      <c r="D2" s="52">
+      <c r="D2" s="48">
         <v>1420</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="49">
         <v>2334628</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="49">
         <v>76534</v>
       </c>
       <c r="H2" s="10">
@@ -4481,30 +4464,30 @@
       <c r="I2" s="10">
         <v>3.5</v>
       </c>
-      <c r="J2" s="54">
+      <c r="J2" s="50">
         <v>150000</v>
       </c>
       <c r="K2" s="9">
         <f>J2*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L2" s="55">
+      <c r="L2" s="51">
         <v>19.399999999999999</v>
       </c>
-      <c r="M2" s="56">
+      <c r="M2" s="52">
         <f>0.1*L2</f>
         <v>1.94</v>
       </c>
-      <c r="N2" s="57">
+      <c r="N2" s="53">
         <v>0</v>
       </c>
       <c r="O2" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P2" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="56">
+      <c r="P2" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="52">
         <f>0.1*P2</f>
         <v>0</v>
       </c>
@@ -4517,31 +4500,31 @@
       <c r="T2" s="10">
         <v>55.300929440000004</v>
       </c>
-      <c r="U2" s="56">
+      <c r="U2" s="52">
         <f>0.1*T2</f>
         <v>5.5300929440000006</v>
       </c>
-      <c r="V2" s="58">
-        <v>0</v>
-      </c>
-      <c r="W2" s="58">
-        <v>0</v>
-      </c>
-      <c r="X2" s="56">
+      <c r="V2" s="54">
+        <v>0</v>
+      </c>
+      <c r="W2" s="54">
+        <v>0</v>
+      </c>
+      <c r="X2" s="52">
         <f>0.1*W2</f>
         <v>0</v>
       </c>
-      <c r="Y2" s="59">
+      <c r="Y2" s="55">
         <v>1E-3</v>
       </c>
-      <c r="Z2" s="56">
+      <c r="Z2" s="52">
         <f>0.1*Y2</f>
         <v>1E-4</v>
       </c>
       <c r="AA2" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AB2" s="58">
+      <c r="AB2" s="54">
         <v>0</v>
       </c>
       <c r="AC2" s="10">
@@ -4550,13 +4533,13 @@
       <c r="AD2" s="10">
         <v>44.249000000000002</v>
       </c>
-      <c r="AE2" s="60">
+      <c r="AE2" s="56">
         <v>0</v>
       </c>
       <c r="AF2" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AG2" s="60">
+      <c r="AG2" s="56">
         <v>0</v>
       </c>
       <c r="AH2" s="10">
@@ -4568,13 +4551,13 @@
       <c r="AJ2" s="10">
         <v>55.300929440000004</v>
       </c>
-      <c r="AK2" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="60">
+      <c r="AK2" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="56">
         <v>1E-3</v>
       </c>
       <c r="AN2" s="10">
@@ -4589,7 +4572,7 @@
       <c r="AQ2" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="AR2" s="60">
+      <c r="AR2" s="56">
         <v>0</v>
       </c>
       <c r="AS2" s="10">
@@ -4640,26 +4623,26 @@
       <c r="BX2" s="23"/>
       <c r="BY2" s="23"/>
     </row>
-    <row r="3" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
-        <v>131</v>
-      </c>
-      <c r="B3" s="50">
+    <row r="3" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="B3" s="46">
         <v>42.129652499999999</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="47">
         <v>13.41337867</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="48">
         <v>1416</v>
       </c>
       <c r="E3" s="10">
         <v>0</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="49">
         <v>2389795</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="49">
         <v>74627</v>
       </c>
       <c r="H3" s="10">
@@ -4668,30 +4651,30 @@
       <c r="I3" s="10">
         <v>3</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="50">
         <v>150000</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ref="K3:K4" si="0">J3*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L3" s="55">
+      <c r="L3" s="51">
         <v>36.61</v>
       </c>
-      <c r="M3" s="56">
+      <c r="M3" s="52">
         <f t="shared" ref="M3:M7" si="1">0.1*L3</f>
         <v>3.661</v>
       </c>
-      <c r="N3" s="57">
+      <c r="N3" s="53">
         <v>0</v>
       </c>
       <c r="O3" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P3" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="56">
+      <c r="P3" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="52">
         <f t="shared" ref="Q3:Q7" si="2">0.1*P3</f>
         <v>0</v>
       </c>
@@ -4704,31 +4687,31 @@
       <c r="T3" s="10">
         <v>54.192184820000001</v>
       </c>
-      <c r="U3" s="56">
+      <c r="U3" s="52">
         <f t="shared" ref="U3:U7" si="3">0.1*T3</f>
         <v>5.4192184820000007</v>
       </c>
-      <c r="V3" s="58">
-        <v>0</v>
-      </c>
-      <c r="W3" s="58">
-        <v>0</v>
-      </c>
-      <c r="X3" s="56">
+      <c r="V3" s="54">
+        <v>0</v>
+      </c>
+      <c r="W3" s="54">
+        <v>0</v>
+      </c>
+      <c r="X3" s="52">
         <f t="shared" ref="X3:X7" si="4">0.1*W3</f>
         <v>0</v>
       </c>
-      <c r="Y3" s="59">
+      <c r="Y3" s="55">
         <v>1E-3</v>
       </c>
-      <c r="Z3" s="56">
+      <c r="Z3" s="52">
         <f t="shared" ref="Z3:Z7" si="5">0.1*Y3</f>
         <v>1E-4</v>
       </c>
       <c r="AA3" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AB3" s="58">
+      <c r="AB3" s="54">
         <v>0</v>
       </c>
       <c r="AC3" s="10">
@@ -4737,13 +4720,13 @@
       <c r="AD3" s="10">
         <v>44.249000000000002</v>
       </c>
-      <c r="AE3" s="60">
+      <c r="AE3" s="56">
         <v>0</v>
       </c>
       <c r="AF3" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AG3" s="60">
+      <c r="AG3" s="56">
         <v>0</v>
       </c>
       <c r="AH3" s="10">
@@ -4755,13 +4738,13 @@
       <c r="AJ3" s="10">
         <v>54.192184820000001</v>
       </c>
-      <c r="AK3" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="60">
+      <c r="AK3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="56">
         <v>1E-3</v>
       </c>
       <c r="AN3" s="10">
@@ -4776,7 +4759,7 @@
       <c r="AQ3" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="AR3" s="60">
+      <c r="AR3" s="56">
         <v>0</v>
       </c>
       <c r="AS3" s="10">
@@ -4827,26 +4810,26 @@
       <c r="BX3" s="23"/>
       <c r="BY3" s="23"/>
     </row>
-    <row r="4" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
-        <v>132</v>
-      </c>
-      <c r="B4" s="50">
+    <row r="4" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="B4" s="46">
         <v>42.129649669999999</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="47">
         <v>13.413381299999999</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="57">
         <v>1381.1</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="49">
         <v>2540835</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="49">
         <v>79038</v>
       </c>
       <c r="H4" s="10">
@@ -4855,30 +4838,30 @@
       <c r="I4" s="10">
         <v>2</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="50">
         <v>150000</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L4" s="55">
+      <c r="L4" s="51">
         <v>25.51</v>
       </c>
-      <c r="M4" s="56">
+      <c r="M4" s="52">
         <f t="shared" si="1"/>
         <v>2.5510000000000002</v>
       </c>
-      <c r="N4" s="57">
+      <c r="N4" s="53">
         <v>0</v>
       </c>
       <c r="O4" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P4" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="56">
+      <c r="P4" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4891,31 +4874,31 @@
       <c r="T4" s="10">
         <v>56.626441120000003</v>
       </c>
-      <c r="U4" s="56">
+      <c r="U4" s="52">
         <f t="shared" si="3"/>
         <v>5.6626441120000006</v>
       </c>
-      <c r="V4" s="58">
-        <v>0</v>
-      </c>
-      <c r="W4" s="58">
-        <v>0</v>
-      </c>
-      <c r="X4" s="56">
+      <c r="V4" s="54">
+        <v>0</v>
+      </c>
+      <c r="W4" s="54">
+        <v>0</v>
+      </c>
+      <c r="X4" s="52">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y4" s="59">
+      <c r="Y4" s="55">
         <v>1E-3</v>
       </c>
-      <c r="Z4" s="56">
+      <c r="Z4" s="52">
         <f t="shared" si="5"/>
         <v>1E-4</v>
       </c>
       <c r="AA4" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AB4" s="58">
+      <c r="AB4" s="54">
         <v>0</v>
       </c>
       <c r="AC4" s="10">
@@ -4924,13 +4907,13 @@
       <c r="AD4" s="10">
         <v>44.249000000000002</v>
       </c>
-      <c r="AE4" s="60">
+      <c r="AE4" s="56">
         <v>0</v>
       </c>
       <c r="AF4" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AG4" s="60">
+      <c r="AG4" s="56">
         <v>0</v>
       </c>
       <c r="AH4" s="10">
@@ -4942,13 +4925,13 @@
       <c r="AJ4" s="10">
         <v>56.626441120000003</v>
       </c>
-      <c r="AK4" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="60">
+      <c r="AK4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="56">
         <v>1E-3</v>
       </c>
       <c r="AN4" s="10">
@@ -4963,7 +4946,7 @@
       <c r="AQ4" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="AR4" s="60">
+      <c r="AR4" s="56">
         <v>0</v>
       </c>
       <c r="AS4" s="10">
@@ -5014,26 +4997,26 @@
       <c r="BX4" s="23"/>
       <c r="BY4" s="23"/>
     </row>
-    <row r="5" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
-        <v>133</v>
-      </c>
-      <c r="B5" s="50">
+    <row r="5" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="B5" s="46">
         <v>42.129283829999999</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="47">
         <v>13.4129775</v>
       </c>
-      <c r="D5" s="61">
+      <c r="D5" s="57">
         <v>1356.7</v>
       </c>
       <c r="E5" s="10">
         <v>0</v>
       </c>
-      <c r="F5" s="53">
+      <c r="F5" s="49">
         <v>1797778</v>
       </c>
-      <c r="G5" s="53">
+      <c r="G5" s="49">
         <v>56888</v>
       </c>
       <c r="H5" s="10">
@@ -5042,30 +5025,30 @@
       <c r="I5" s="10">
         <v>2.8</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="50">
         <v>150000</v>
       </c>
       <c r="K5" s="9">
         <f>J5*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="51">
         <v>28.01</v>
       </c>
-      <c r="M5" s="56">
+      <c r="M5" s="52">
         <f t="shared" si="1"/>
         <v>2.8010000000000002</v>
       </c>
-      <c r="N5" s="57">
+      <c r="N5" s="53">
         <v>0</v>
       </c>
       <c r="O5" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P5" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="56">
+      <c r="P5" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5078,31 +5061,31 @@
       <c r="T5" s="10">
         <v>55.755874379999995</v>
       </c>
-      <c r="U5" s="56">
+      <c r="U5" s="52">
         <f t="shared" si="3"/>
         <v>5.5755874379999995</v>
       </c>
-      <c r="V5" s="58">
-        <v>0</v>
-      </c>
-      <c r="W5" s="58">
-        <v>0</v>
-      </c>
-      <c r="X5" s="56">
+      <c r="V5" s="54">
+        <v>0</v>
+      </c>
+      <c r="W5" s="54">
+        <v>0</v>
+      </c>
+      <c r="X5" s="52">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y5" s="59">
+      <c r="Y5" s="55">
         <v>1E-3</v>
       </c>
-      <c r="Z5" s="56">
+      <c r="Z5" s="52">
         <f t="shared" si="5"/>
         <v>1E-4</v>
       </c>
       <c r="AA5" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AB5" s="58">
+      <c r="AB5" s="54">
         <v>0</v>
       </c>
       <c r="AC5" s="10">
@@ -5111,13 +5094,13 @@
       <c r="AD5" s="10">
         <v>44.249000000000002</v>
       </c>
-      <c r="AE5" s="60">
+      <c r="AE5" s="56">
         <v>0</v>
       </c>
       <c r="AF5" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AG5" s="60">
+      <c r="AG5" s="56">
         <v>0</v>
       </c>
       <c r="AH5" s="10">
@@ -5129,13 +5112,13 @@
       <c r="AJ5" s="10">
         <v>55.755874379999995</v>
       </c>
-      <c r="AK5" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="60">
+      <c r="AK5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="56">
         <v>1E-3</v>
       </c>
       <c r="AN5" s="10">
@@ -5150,7 +5133,7 @@
       <c r="AQ5" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="AR5" s="60">
+      <c r="AR5" s="56">
         <v>0</v>
       </c>
       <c r="AS5" s="10">
@@ -5201,26 +5184,26 @@
       <c r="BX5" s="23"/>
       <c r="BY5" s="23"/>
     </row>
-    <row r="6" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
-        <v>134</v>
-      </c>
-      <c r="B6" s="50">
+    <row r="6" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="46">
         <v>42.128590000000003</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="47">
         <v>13.413190500000001</v>
       </c>
-      <c r="D6" s="61">
+      <c r="D6" s="57">
         <v>1305</v>
       </c>
       <c r="E6" s="10">
         <v>0</v>
       </c>
-      <c r="F6" s="53">
+      <c r="F6" s="49">
         <v>3041120</v>
       </c>
-      <c r="G6" s="53">
+      <c r="G6" s="49">
         <v>84229</v>
       </c>
       <c r="H6" s="10">
@@ -5229,30 +5212,30 @@
       <c r="I6" s="10">
         <v>3</v>
       </c>
-      <c r="J6" s="54">
+      <c r="J6" s="50">
         <v>150000</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" ref="K6:K7" si="6">J6*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L6" s="55">
+      <c r="L6" s="51">
         <v>20.46</v>
       </c>
-      <c r="M6" s="56">
+      <c r="M6" s="52">
         <f t="shared" si="1"/>
         <v>2.0460000000000003</v>
       </c>
-      <c r="N6" s="57">
+      <c r="N6" s="53">
         <v>0</v>
       </c>
       <c r="O6" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P6" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="56">
+      <c r="P6" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5265,31 +5248,31 @@
       <c r="T6" s="10">
         <v>57.720492039999996</v>
       </c>
-      <c r="U6" s="56">
+      <c r="U6" s="52">
         <f t="shared" si="3"/>
         <v>5.772049204</v>
       </c>
-      <c r="V6" s="58">
-        <v>0</v>
-      </c>
-      <c r="W6" s="58">
-        <v>0</v>
-      </c>
-      <c r="X6" s="56">
+      <c r="V6" s="54">
+        <v>0</v>
+      </c>
+      <c r="W6" s="54">
+        <v>0</v>
+      </c>
+      <c r="X6" s="52">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y6" s="59">
+      <c r="Y6" s="55">
         <v>1E-3</v>
       </c>
-      <c r="Z6" s="56">
+      <c r="Z6" s="52">
         <f t="shared" si="5"/>
         <v>1E-4</v>
       </c>
       <c r="AA6" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AB6" s="58">
+      <c r="AB6" s="54">
         <v>0</v>
       </c>
       <c r="AC6" s="10">
@@ -5298,13 +5281,13 @@
       <c r="AD6" s="10">
         <v>44.249000000000002</v>
       </c>
-      <c r="AE6" s="60">
+      <c r="AE6" s="56">
         <v>0</v>
       </c>
       <c r="AF6" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AG6" s="60">
+      <c r="AG6" s="56">
         <v>0</v>
       </c>
       <c r="AH6" s="10">
@@ -5316,13 +5299,13 @@
       <c r="AJ6" s="10">
         <v>57.720492039999996</v>
       </c>
-      <c r="AK6" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="60">
+      <c r="AK6" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="56">
         <v>1E-3</v>
       </c>
       <c r="AN6" s="10">
@@ -5337,7 +5320,7 @@
       <c r="AQ6" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="AR6" s="60">
+      <c r="AR6" s="56">
         <v>0</v>
       </c>
       <c r="AS6" s="10">
@@ -5388,26 +5371,26 @@
       <c r="BX6" s="23"/>
       <c r="BY6" s="23"/>
     </row>
-    <row r="7" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
-        <v>135</v>
-      </c>
-      <c r="B7" s="50">
+    <row r="7" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B7" s="46">
         <v>42.128399330000001</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="47">
         <v>13.413185670000001</v>
       </c>
-      <c r="D7" s="61">
+      <c r="D7" s="57">
         <v>1302.2</v>
       </c>
       <c r="E7" s="10">
         <v>0</v>
       </c>
-      <c r="F7" s="53">
+      <c r="F7" s="49">
         <v>3027645</v>
       </c>
-      <c r="G7" s="53">
+      <c r="G7" s="49">
         <v>83462</v>
       </c>
       <c r="H7" s="10">
@@ -5416,30 +5399,30 @@
       <c r="I7" s="10">
         <v>2.5</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="50">
         <v>150000</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" si="6"/>
         <v>15000</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="51">
         <v>21.09</v>
       </c>
-      <c r="M7" s="56">
+      <c r="M7" s="52">
         <f t="shared" si="1"/>
         <v>2.109</v>
       </c>
-      <c r="N7" s="57">
+      <c r="N7" s="53">
         <v>0</v>
       </c>
       <c r="O7" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="P7" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="56">
+      <c r="P7" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="52">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -5452,31 +5435,31 @@
       <c r="T7" s="10">
         <v>55.250551040000005</v>
       </c>
-      <c r="U7" s="56">
+      <c r="U7" s="52">
         <f t="shared" si="3"/>
         <v>5.5250551040000007</v>
       </c>
-      <c r="V7" s="58">
-        <v>0</v>
-      </c>
-      <c r="W7" s="58">
-        <v>0</v>
-      </c>
-      <c r="X7" s="56">
+      <c r="V7" s="54">
+        <v>0</v>
+      </c>
+      <c r="W7" s="54">
+        <v>0</v>
+      </c>
+      <c r="X7" s="52">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="Y7" s="59">
+      <c r="Y7" s="55">
         <v>1E-3</v>
       </c>
-      <c r="Z7" s="56">
+      <c r="Z7" s="52">
         <f t="shared" si="5"/>
         <v>1E-4</v>
       </c>
       <c r="AA7" s="10">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="AB7" s="58">
+      <c r="AB7" s="54">
         <v>0</v>
       </c>
       <c r="AC7" s="10">
@@ -5485,13 +5468,13 @@
       <c r="AD7" s="10">
         <v>44.249000000000002</v>
       </c>
-      <c r="AE7" s="60">
+      <c r="AE7" s="56">
         <v>0</v>
       </c>
       <c r="AF7" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="AG7" s="60">
+      <c r="AG7" s="56">
         <v>0</v>
       </c>
       <c r="AH7" s="10">
@@ -5503,13 +5486,13 @@
       <c r="AJ7" s="10">
         <v>55.250551040000005</v>
       </c>
-      <c r="AK7" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="60">
+      <c r="AK7" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="56">
         <v>1E-3</v>
       </c>
       <c r="AN7" s="10">
@@ -5524,7 +5507,7 @@
       <c r="AQ7" s="10">
         <v>1.6E-2</v>
       </c>
-      <c r="AR7" s="60">
+      <c r="AR7" s="56">
         <v>0</v>
       </c>
       <c r="AS7" s="10">
@@ -5576,49 +5559,49 @@
       <c r="BY7" s="23"/>
     </row>
     <row r="8" spans="1:77" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="62"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="60"/>
       <c r="E8" s="20"/>
       <c r="F8" s="20"/>
       <c r="G8" s="20"/>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
-      <c r="J8" s="65"/>
+      <c r="J8" s="61"/>
       <c r="K8" s="21"/>
-      <c r="L8" s="66"/>
+      <c r="L8" s="62"/>
       <c r="M8" s="21"/>
-      <c r="N8" s="67"/>
+      <c r="N8" s="63"/>
       <c r="O8" s="20"/>
-      <c r="P8" s="68"/>
-      <c r="Q8" s="68"/>
+      <c r="P8" s="64"/>
+      <c r="Q8" s="64"/>
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
       <c r="U8" s="21"/>
-      <c r="V8" s="69"/>
-      <c r="W8" s="69"/>
-      <c r="X8" s="69"/>
-      <c r="Y8" s="69"/>
-      <c r="Z8" s="69"/>
+      <c r="V8" s="65"/>
+      <c r="W8" s="65"/>
+      <c r="X8" s="65"/>
+      <c r="Y8" s="65"/>
+      <c r="Z8" s="65"/>
       <c r="AA8" s="20"/>
-      <c r="AB8" s="69"/>
+      <c r="AB8" s="65"/>
       <c r="AC8" s="20"/>
       <c r="AD8" s="20"/>
-      <c r="AE8" s="69"/>
+      <c r="AE8" s="65"/>
       <c r="AF8" s="20"/>
-      <c r="AG8" s="68"/>
+      <c r="AG8" s="64"/>
       <c r="AH8" s="20"/>
       <c r="AI8" s="20"/>
       <c r="AJ8" s="20"/>
-      <c r="AK8" s="69"/>
-      <c r="AL8" s="69"/>
-      <c r="AM8" s="69"/>
+      <c r="AK8" s="65"/>
+      <c r="AL8" s="65"/>
+      <c r="AM8" s="65"/>
       <c r="AN8" s="20"/>
       <c r="AO8" s="20"/>
       <c r="AP8" s="20"/>
       <c r="AQ8" s="20"/>
-      <c r="AR8" s="69"/>
+      <c r="AR8" s="65"/>
       <c r="AS8" s="20"/>
       <c r="AT8" s="20"/>
       <c r="AU8" s="20"/>
@@ -5628,49 +5611,49 @@
       <c r="AY8" s="20"/>
     </row>
     <row r="9" spans="1:77" s="23" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="62"/>
-      <c r="C9" s="63"/>
-      <c r="D9" s="64"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="60"/>
       <c r="E9" s="20"/>
       <c r="F9" s="20"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="65"/>
+      <c r="J9" s="61"/>
       <c r="K9" s="21"/>
-      <c r="L9" s="66"/>
+      <c r="L9" s="62"/>
       <c r="M9" s="21"/>
-      <c r="N9" s="67"/>
+      <c r="N9" s="63"/>
       <c r="O9" s="20"/>
-      <c r="P9" s="68"/>
-      <c r="Q9" s="68"/>
+      <c r="P9" s="64"/>
+      <c r="Q9" s="64"/>
       <c r="R9" s="20"/>
       <c r="S9" s="20"/>
       <c r="T9" s="20"/>
       <c r="U9" s="21"/>
-      <c r="V9" s="69"/>
-      <c r="W9" s="69"/>
-      <c r="X9" s="69"/>
-      <c r="Y9" s="69"/>
-      <c r="Z9" s="69"/>
+      <c r="V9" s="65"/>
+      <c r="W9" s="65"/>
+      <c r="X9" s="65"/>
+      <c r="Y9" s="65"/>
+      <c r="Z9" s="65"/>
       <c r="AA9" s="20"/>
-      <c r="AB9" s="69"/>
+      <c r="AB9" s="65"/>
       <c r="AC9" s="20"/>
       <c r="AD9" s="20"/>
-      <c r="AE9" s="69"/>
+      <c r="AE9" s="65"/>
       <c r="AF9" s="20"/>
-      <c r="AG9" s="68"/>
+      <c r="AG9" s="64"/>
       <c r="AH9" s="20"/>
       <c r="AI9" s="20"/>
       <c r="AJ9" s="20"/>
-      <c r="AK9" s="69"/>
-      <c r="AL9" s="69"/>
-      <c r="AM9" s="69"/>
+      <c r="AK9" s="65"/>
+      <c r="AL9" s="65"/>
+      <c r="AM9" s="65"/>
       <c r="AN9" s="20"/>
       <c r="AO9" s="20"/>
       <c r="AP9" s="20"/>
       <c r="AQ9" s="20"/>
-      <c r="AR9" s="69"/>
+      <c r="AR9" s="65"/>
       <c r="AS9" s="20"/>
       <c r="AT9" s="20"/>
       <c r="AU9" s="20"/>
@@ -5681,8 +5664,8 @@
     </row>
     <row r="10" spans="1:77" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
@@ -8308,7 +8291,7 @@
     <col min="24" max="24" width="13.83203125" style="2" customWidth="1"/>
     <col min="25" max="25" width="13.83203125" style="3" customWidth="1"/>
     <col min="26" max="29" width="13.83203125" style="6" customWidth="1"/>
-    <col min="30" max="43" width="13.83203125" style="71" customWidth="1"/>
+    <col min="30" max="43" width="13.83203125" style="67" customWidth="1"/>
     <col min="44" max="46" width="13.83203125" style="10" customWidth="1"/>
     <col min="47" max="47" width="13.83203125" style="8" customWidth="1"/>
     <col min="48" max="49" width="13.83203125" style="10" customWidth="1"/>
@@ -8407,7 +8390,7 @@
       <c r="AD1" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="48" t="s">
+      <c r="AE1" s="44" t="s">
         <v>22</v>
       </c>
       <c r="AF1" s="11" t="s">
@@ -8497,17 +8480,17 @@
       <c r="BX1" s="39"/>
       <c r="BY1" s="39"/>
     </row>
-    <row r="2" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="B2" s="50">
+    <row r="2" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="B2" s="46">
         <v>42.194646169999999</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="47">
         <v>13.71451233</v>
       </c>
-      <c r="D2" s="52">
+      <c r="D2" s="48">
         <v>1060</v>
       </c>
       <c r="E2" s="10">
@@ -8525,30 +8508,30 @@
       <c r="I2" s="10">
         <v>4.5</v>
       </c>
-      <c r="J2" s="54">
+      <c r="J2" s="50">
         <v>150000</v>
       </c>
       <c r="K2" s="9">
         <f t="shared" ref="K2:K9" si="0">J2*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L2" s="55">
+      <c r="L2" s="51">
         <v>3.81</v>
       </c>
       <c r="M2" s="9">
         <f>L2*0.1</f>
         <v>0.38100000000000001</v>
       </c>
-      <c r="N2" s="57">
+      <c r="N2" s="53">
         <v>0</v>
       </c>
       <c r="O2" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P2" s="58">
+      <c r="P2" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q2" s="58">
+      <c r="Q2" s="54">
         <f>0.1*P2</f>
         <v>1E-3</v>
       </c>
@@ -8558,32 +8541,32 @@
       <c r="S2" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T2" s="72">
+      <c r="T2" s="68">
         <v>55.123677503686004</v>
       </c>
       <c r="U2" s="9">
         <f>T2*0.1</f>
         <v>5.5123677503686004</v>
       </c>
-      <c r="V2" s="60">
-        <v>0</v>
-      </c>
-      <c r="W2" s="60">
-        <v>0</v>
-      </c>
-      <c r="X2" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="60">
+      <c r="V2" s="56">
+        <v>0</v>
+      </c>
+      <c r="W2" s="56">
+        <v>0</v>
+      </c>
+      <c r="X2" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="56">
         <v>0</v>
       </c>
       <c r="AA2" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB2" s="60">
+      <c r="AB2" s="56">
         <v>0</v>
       </c>
       <c r="AC2" s="10">
@@ -8592,13 +8575,13 @@
       <c r="AD2" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE2" s="60">
+      <c r="AE2" s="56">
         <v>0</v>
       </c>
       <c r="AF2" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG2" s="58">
+      <c r="AG2" s="54">
         <v>0.01</v>
       </c>
       <c r="AH2" s="10">
@@ -8607,16 +8590,16 @@
       <c r="AI2" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ2" s="72">
+      <c r="AJ2" s="68">
         <v>55.123677503686004</v>
       </c>
-      <c r="AK2" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="60">
+      <c r="AK2" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="56">
         <v>0</v>
       </c>
       <c r="AN2" s="10">
@@ -8631,7 +8614,7 @@
       <c r="AQ2" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR2" s="60">
+      <c r="AR2" s="56">
         <v>0</v>
       </c>
       <c r="AS2" s="10">
@@ -8682,17 +8665,17 @@
       <c r="BX2" s="23"/>
       <c r="BY2" s="23"/>
     </row>
-    <row r="3" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="B3" s="50">
+    <row r="3" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="B3" s="46">
         <v>42.193992170000001</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="47">
         <v>13.71415133</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="48">
         <v>1026</v>
       </c>
       <c r="E3" s="10">
@@ -8710,30 +8693,30 @@
       <c r="I3" s="10">
         <v>3</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="50">
         <v>150000</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L3" s="55">
+      <c r="L3" s="51">
         <v>3.32</v>
       </c>
       <c r="M3" s="9">
         <f t="shared" ref="M3:M9" si="1">L3*0.1</f>
         <v>0.33200000000000002</v>
       </c>
-      <c r="N3" s="57">
+      <c r="N3" s="53">
         <v>0</v>
       </c>
       <c r="O3" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P3" s="58">
+      <c r="P3" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q3" s="58">
+      <c r="Q3" s="54">
         <f t="shared" ref="Q3:Q9" si="2">0.1*P3</f>
         <v>1E-3</v>
       </c>
@@ -8743,32 +8726,32 @@
       <c r="S3" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T3" s="72">
+      <c r="T3" s="68">
         <v>55.615599083759996</v>
       </c>
       <c r="U3" s="9">
         <f t="shared" ref="U3:U9" si="3">T3*0.1</f>
         <v>5.5615599083760001</v>
       </c>
-      <c r="V3" s="60">
-        <v>0</v>
-      </c>
-      <c r="W3" s="60">
-        <v>0</v>
-      </c>
-      <c r="X3" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="60">
+      <c r="V3" s="56">
+        <v>0</v>
+      </c>
+      <c r="W3" s="56">
+        <v>0</v>
+      </c>
+      <c r="X3" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="56">
         <v>0</v>
       </c>
       <c r="AA3" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB3" s="60">
+      <c r="AB3" s="56">
         <v>0</v>
       </c>
       <c r="AC3" s="10">
@@ -8777,13 +8760,13 @@
       <c r="AD3" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE3" s="60">
+      <c r="AE3" s="56">
         <v>0</v>
       </c>
       <c r="AF3" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG3" s="58">
+      <c r="AG3" s="54">
         <v>0.01</v>
       </c>
       <c r="AH3" s="10">
@@ -8792,16 +8775,16 @@
       <c r="AI3" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ3" s="72">
+      <c r="AJ3" s="68">
         <v>55.615599083759996</v>
       </c>
-      <c r="AK3" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="60">
+      <c r="AK3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="56">
         <v>0</v>
       </c>
       <c r="AN3" s="10">
@@ -8816,7 +8799,7 @@
       <c r="AQ3" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR3" s="60">
+      <c r="AR3" s="56">
         <v>0</v>
       </c>
       <c r="AS3" s="10">
@@ -8867,17 +8850,17 @@
       <c r="BX3" s="23"/>
       <c r="BY3" s="23"/>
     </row>
-    <row r="4" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
-        <v>138</v>
-      </c>
-      <c r="B4" s="50">
+    <row r="4" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>135</v>
+      </c>
+      <c r="B4" s="46">
         <v>42.193688999999999</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="47">
         <v>13.713477170000001</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="57">
         <v>996.3</v>
       </c>
       <c r="E4" s="10">
@@ -8895,30 +8878,30 @@
       <c r="I4" s="10">
         <v>3</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="50">
         <v>150000</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L4" s="55">
+      <c r="L4" s="51">
         <v>5.58</v>
       </c>
       <c r="M4" s="9">
         <f t="shared" si="1"/>
         <v>0.55800000000000005</v>
       </c>
-      <c r="N4" s="57">
+      <c r="N4" s="53">
         <v>0</v>
       </c>
       <c r="O4" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P4" s="58">
+      <c r="P4" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q4" s="58">
+      <c r="Q4" s="54">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
@@ -8928,32 +8911,32 @@
       <c r="S4" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T4" s="72">
+      <c r="T4" s="68">
         <v>54.743000834780005</v>
       </c>
       <c r="U4" s="9">
         <f t="shared" si="3"/>
         <v>5.4743000834780009</v>
       </c>
-      <c r="V4" s="60">
-        <v>0</v>
-      </c>
-      <c r="W4" s="60">
-        <v>0</v>
-      </c>
-      <c r="X4" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="60">
+      <c r="V4" s="56">
+        <v>0</v>
+      </c>
+      <c r="W4" s="56">
+        <v>0</v>
+      </c>
+      <c r="X4" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="56">
         <v>0</v>
       </c>
       <c r="AA4" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB4" s="60">
+      <c r="AB4" s="56">
         <v>0</v>
       </c>
       <c r="AC4" s="10">
@@ -8962,13 +8945,13 @@
       <c r="AD4" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE4" s="60">
+      <c r="AE4" s="56">
         <v>0</v>
       </c>
       <c r="AF4" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG4" s="58">
+      <c r="AG4" s="54">
         <v>0.01</v>
       </c>
       <c r="AH4" s="10">
@@ -8977,16 +8960,16 @@
       <c r="AI4" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ4" s="72">
+      <c r="AJ4" s="68">
         <v>54.743000834780005</v>
       </c>
-      <c r="AK4" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="60">
+      <c r="AK4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="56">
         <v>0</v>
       </c>
       <c r="AN4" s="10">
@@ -9001,7 +8984,7 @@
       <c r="AQ4" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR4" s="60">
+      <c r="AR4" s="56">
         <v>0</v>
       </c>
       <c r="AS4" s="10">
@@ -9052,17 +9035,17 @@
       <c r="BX4" s="23"/>
       <c r="BY4" s="23"/>
     </row>
-    <row r="5" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="49" t="s">
-        <v>139</v>
-      </c>
-      <c r="B5" s="50">
+    <row r="5" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="45" t="s">
+        <v>136</v>
+      </c>
+      <c r="B5" s="46">
         <v>42.193133600000003</v>
       </c>
-      <c r="C5" s="51">
+      <c r="C5" s="47">
         <v>13.7128371</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="48">
         <v>951</v>
       </c>
       <c r="E5" s="10">
@@ -9080,30 +9063,30 @@
       <c r="I5" s="10">
         <v>3</v>
       </c>
-      <c r="J5" s="54">
+      <c r="J5" s="50">
         <v>150000</v>
       </c>
       <c r="K5" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L5" s="55">
+      <c r="L5" s="51">
         <v>5.51</v>
       </c>
       <c r="M5" s="9">
         <f t="shared" si="1"/>
         <v>0.55100000000000005</v>
       </c>
-      <c r="N5" s="57">
+      <c r="N5" s="53">
         <v>0</v>
       </c>
       <c r="O5" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P5" s="58">
+      <c r="P5" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q5" s="58">
+      <c r="Q5" s="54">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
@@ -9113,32 +9096,32 @@
       <c r="S5" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T5" s="72">
+      <c r="T5" s="68">
         <v>54.800369671594005</v>
       </c>
       <c r="U5" s="9">
         <f t="shared" si="3"/>
         <v>5.4800369671594007</v>
       </c>
-      <c r="V5" s="60">
-        <v>0</v>
-      </c>
-      <c r="W5" s="60">
-        <v>0</v>
-      </c>
-      <c r="X5" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="60">
+      <c r="V5" s="56">
+        <v>0</v>
+      </c>
+      <c r="W5" s="56">
+        <v>0</v>
+      </c>
+      <c r="X5" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="56">
         <v>0</v>
       </c>
       <c r="AA5" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB5" s="60">
+      <c r="AB5" s="56">
         <v>0</v>
       </c>
       <c r="AC5" s="10">
@@ -9147,13 +9130,13 @@
       <c r="AD5" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE5" s="60">
+      <c r="AE5" s="56">
         <v>0</v>
       </c>
       <c r="AF5" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG5" s="58">
+      <c r="AG5" s="54">
         <v>0.01</v>
       </c>
       <c r="AH5" s="10">
@@ -9162,16 +9145,16 @@
       <c r="AI5" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ5" s="72">
+      <c r="AJ5" s="68">
         <v>54.800369671594005</v>
       </c>
-      <c r="AK5" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="60">
+      <c r="AK5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="56">
         <v>0</v>
       </c>
       <c r="AN5" s="10">
@@ -9186,7 +9169,7 @@
       <c r="AQ5" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR5" s="60">
+      <c r="AR5" s="56">
         <v>0</v>
       </c>
       <c r="AS5" s="10">
@@ -9237,17 +9220,17 @@
       <c r="BX5" s="23"/>
       <c r="BY5" s="23"/>
     </row>
-    <row r="6" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="49" t="s">
-        <v>140</v>
-      </c>
-      <c r="B6" s="50">
+    <row r="6" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="45" t="s">
+        <v>137</v>
+      </c>
+      <c r="B6" s="46">
         <v>42.19276</v>
       </c>
-      <c r="C6" s="51">
+      <c r="C6" s="47">
         <v>13.712339999999999</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="48">
         <v>917</v>
       </c>
       <c r="E6" s="10">
@@ -9265,30 +9248,30 @@
       <c r="I6" s="10">
         <v>2.5</v>
       </c>
-      <c r="J6" s="54">
+      <c r="J6" s="50">
         <v>150000</v>
       </c>
       <c r="K6" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L6" s="55">
+      <c r="L6" s="51">
         <v>5.55</v>
       </c>
       <c r="M6" s="9">
         <f t="shared" si="1"/>
         <v>0.55500000000000005</v>
       </c>
-      <c r="N6" s="57">
+      <c r="N6" s="53">
         <v>0</v>
       </c>
       <c r="O6" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P6" s="58">
+      <c r="P6" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q6" s="58">
+      <c r="Q6" s="54">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
@@ -9298,32 +9281,32 @@
       <c r="S6" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T6" s="72">
+      <c r="T6" s="68">
         <v>55.50736792043201</v>
       </c>
       <c r="U6" s="9">
         <f t="shared" si="3"/>
         <v>5.5507367920432014</v>
       </c>
-      <c r="V6" s="60">
-        <v>0</v>
-      </c>
-      <c r="W6" s="60">
-        <v>0</v>
-      </c>
-      <c r="X6" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="60">
+      <c r="V6" s="56">
+        <v>0</v>
+      </c>
+      <c r="W6" s="56">
+        <v>0</v>
+      </c>
+      <c r="X6" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="56">
         <v>0</v>
       </c>
       <c r="AA6" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB6" s="60">
+      <c r="AB6" s="56">
         <v>0</v>
       </c>
       <c r="AC6" s="10">
@@ -9332,13 +9315,13 @@
       <c r="AD6" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE6" s="60">
+      <c r="AE6" s="56">
         <v>0</v>
       </c>
       <c r="AF6" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG6" s="58">
+      <c r="AG6" s="54">
         <v>0.01</v>
       </c>
       <c r="AH6" s="10">
@@ -9347,16 +9330,16 @@
       <c r="AI6" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ6" s="72">
+      <c r="AJ6" s="68">
         <v>55.50736792043201</v>
       </c>
-      <c r="AK6" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="60">
+      <c r="AK6" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="56">
         <v>0</v>
       </c>
       <c r="AN6" s="10">
@@ -9371,7 +9354,7 @@
       <c r="AQ6" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR6" s="60">
+      <c r="AR6" s="56">
         <v>0</v>
       </c>
       <c r="AS6" s="10">
@@ -9422,17 +9405,17 @@
       <c r="BX6" s="23"/>
       <c r="BY6" s="23"/>
     </row>
-    <row r="7" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="49" t="s">
-        <v>141</v>
-      </c>
-      <c r="B7" s="50">
+    <row r="7" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="B7" s="46">
         <v>42.192590000000003</v>
       </c>
-      <c r="C7" s="51">
+      <c r="C7" s="47">
         <v>13.71223</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="48">
         <v>895</v>
       </c>
       <c r="E7" s="10">
@@ -9450,30 +9433,30 @@
       <c r="I7" s="10">
         <v>3</v>
       </c>
-      <c r="J7" s="54">
+      <c r="J7" s="50">
         <v>150000</v>
       </c>
       <c r="K7" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L7" s="55">
+      <c r="L7" s="51">
         <v>12.79</v>
       </c>
       <c r="M7" s="9">
         <f t="shared" si="1"/>
         <v>1.2789999999999999</v>
       </c>
-      <c r="N7" s="57">
+      <c r="N7" s="53">
         <v>0</v>
       </c>
       <c r="O7" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P7" s="58">
+      <c r="P7" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q7" s="58">
+      <c r="Q7" s="54">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
@@ -9483,32 +9466,32 @@
       <c r="S7" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T7" s="72">
+      <c r="T7" s="68">
         <v>55.37710351197201</v>
       </c>
       <c r="U7" s="9">
         <f t="shared" si="3"/>
         <v>5.5377103511972017</v>
       </c>
-      <c r="V7" s="60">
-        <v>0</v>
-      </c>
-      <c r="W7" s="60">
-        <v>0</v>
-      </c>
-      <c r="X7" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="60">
+      <c r="V7" s="56">
+        <v>0</v>
+      </c>
+      <c r="W7" s="56">
+        <v>0</v>
+      </c>
+      <c r="X7" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="56">
         <v>0</v>
       </c>
       <c r="AA7" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB7" s="60">
+      <c r="AB7" s="56">
         <v>0</v>
       </c>
       <c r="AC7" s="10">
@@ -9517,13 +9500,13 @@
       <c r="AD7" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE7" s="60">
+      <c r="AE7" s="56">
         <v>0</v>
       </c>
       <c r="AF7" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG7" s="58">
+      <c r="AG7" s="54">
         <v>0.01</v>
       </c>
       <c r="AH7" s="10">
@@ -9532,16 +9515,16 @@
       <c r="AI7" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ7" s="72">
+      <c r="AJ7" s="68">
         <v>55.37710351197201</v>
       </c>
-      <c r="AK7" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="60">
+      <c r="AK7" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="56">
         <v>0</v>
       </c>
       <c r="AN7" s="10">
@@ -9556,7 +9539,7 @@
       <c r="AQ7" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR7" s="60">
+      <c r="AR7" s="56">
         <v>0</v>
       </c>
       <c r="AS7" s="10">
@@ -9607,17 +9590,17 @@
       <c r="BX7" s="23"/>
       <c r="BY7" s="23"/>
     </row>
-    <row r="8" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="49" t="s">
-        <v>142</v>
-      </c>
-      <c r="B8" s="50">
+    <row r="8" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="B8" s="46">
         <v>42.192329999999998</v>
       </c>
-      <c r="C8" s="51">
+      <c r="C8" s="47">
         <v>13.712059999999999</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="48">
         <v>888</v>
       </c>
       <c r="E8" s="10">
@@ -9635,30 +9618,30 @@
       <c r="I8" s="10">
         <v>2</v>
       </c>
-      <c r="J8" s="54">
+      <c r="J8" s="50">
         <v>150000</v>
       </c>
       <c r="K8" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L8" s="55">
+      <c r="L8" s="51">
         <v>18.23</v>
       </c>
       <c r="M8" s="9">
         <f t="shared" si="1"/>
         <v>1.8230000000000002</v>
       </c>
-      <c r="N8" s="57">
+      <c r="N8" s="53">
         <v>0</v>
       </c>
       <c r="O8" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P8" s="58">
+      <c r="P8" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q8" s="58">
+      <c r="Q8" s="54">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
@@ -9668,32 +9651,32 @@
       <c r="S8" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T8" s="72">
+      <c r="T8" s="68">
         <v>52.507336915268006</v>
       </c>
       <c r="U8" s="9">
         <f t="shared" si="3"/>
         <v>5.2507336915268006</v>
       </c>
-      <c r="V8" s="60">
-        <v>0</v>
-      </c>
-      <c r="W8" s="60">
-        <v>0</v>
-      </c>
-      <c r="X8" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="60">
+      <c r="V8" s="56">
+        <v>0</v>
+      </c>
+      <c r="W8" s="56">
+        <v>0</v>
+      </c>
+      <c r="X8" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="56">
         <v>0</v>
       </c>
       <c r="AA8" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB8" s="60">
+      <c r="AB8" s="56">
         <v>0</v>
       </c>
       <c r="AC8" s="10">
@@ -9702,13 +9685,13 @@
       <c r="AD8" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE8" s="60">
+      <c r="AE8" s="56">
         <v>0</v>
       </c>
       <c r="AF8" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG8" s="58">
+      <c r="AG8" s="54">
         <v>0.01</v>
       </c>
       <c r="AH8" s="10">
@@ -9717,16 +9700,16 @@
       <c r="AI8" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ8" s="72">
+      <c r="AJ8" s="68">
         <v>52.507336915268006</v>
       </c>
-      <c r="AK8" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="60">
+      <c r="AK8" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="56">
         <v>0</v>
       </c>
       <c r="AN8" s="10">
@@ -9741,7 +9724,7 @@
       <c r="AQ8" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR8" s="60">
+      <c r="AR8" s="56">
         <v>0</v>
       </c>
       <c r="AS8" s="10">
@@ -9792,17 +9775,17 @@
       <c r="BX8" s="23"/>
       <c r="BY8" s="23"/>
     </row>
-    <row r="9" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="49" t="s">
-        <v>143</v>
-      </c>
-      <c r="B9" s="50">
+    <row r="9" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="B9" s="46">
         <v>42.192039999999999</v>
       </c>
-      <c r="C9" s="51">
+      <c r="C9" s="47">
         <v>13.711650000000001</v>
       </c>
-      <c r="D9" s="52">
+      <c r="D9" s="48">
         <v>859</v>
       </c>
       <c r="E9" s="10">
@@ -9820,30 +9803,30 @@
       <c r="I9" s="10">
         <v>3.8</v>
       </c>
-      <c r="J9" s="54">
+      <c r="J9" s="50">
         <v>150000</v>
       </c>
       <c r="K9" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L9" s="55">
+      <c r="L9" s="51">
         <v>35.19</v>
       </c>
       <c r="M9" s="9">
         <f t="shared" si="1"/>
         <v>3.5190000000000001</v>
       </c>
-      <c r="N9" s="57">
+      <c r="N9" s="53">
         <v>0</v>
       </c>
       <c r="O9" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="P9" s="58">
+      <c r="P9" s="54">
         <v>0.01</v>
       </c>
-      <c r="Q9" s="58">
+      <c r="Q9" s="54">
         <f t="shared" si="2"/>
         <v>1E-3</v>
       </c>
@@ -9853,32 +9836,32 @@
       <c r="S9" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="T9" s="72">
+      <c r="T9" s="68">
         <v>54.824062675096002</v>
       </c>
       <c r="U9" s="9">
         <f t="shared" si="3"/>
         <v>5.4824062675096004</v>
       </c>
-      <c r="V9" s="60">
-        <v>0</v>
-      </c>
-      <c r="W9" s="60">
-        <v>0</v>
-      </c>
-      <c r="X9" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="60">
+      <c r="V9" s="56">
+        <v>0</v>
+      </c>
+      <c r="W9" s="56">
+        <v>0</v>
+      </c>
+      <c r="X9" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="56">
         <v>0</v>
       </c>
       <c r="AA9" s="10">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="AB9" s="60">
+      <c r="AB9" s="56">
         <v>0</v>
       </c>
       <c r="AC9" s="10">
@@ -9887,13 +9870,13 @@
       <c r="AD9" s="10">
         <v>43.948999999999998</v>
       </c>
-      <c r="AE9" s="60">
+      <c r="AE9" s="56">
         <v>0</v>
       </c>
       <c r="AF9" s="10">
         <v>3.5999999999999997E-2</v>
       </c>
-      <c r="AG9" s="58">
+      <c r="AG9" s="54">
         <v>0.01</v>
       </c>
       <c r="AH9" s="10">
@@ -9902,16 +9885,16 @@
       <c r="AI9" s="10">
         <v>0.38400000000000001</v>
       </c>
-      <c r="AJ9" s="72">
+      <c r="AJ9" s="68">
         <v>54.824062675096002</v>
       </c>
-      <c r="AK9" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="60">
+      <c r="AK9" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="56">
         <v>0</v>
       </c>
       <c r="AN9" s="10">
@@ -9926,7 +9909,7 @@
       <c r="AQ9" s="10">
         <v>2.1000000000000001E-2</v>
       </c>
-      <c r="AR9" s="60">
+      <c r="AR9" s="56">
         <v>0</v>
       </c>
       <c r="AS9" s="10">
@@ -9979,8 +9962,8 @@
     </row>
     <row r="10" spans="1:77" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
-      <c r="B10" s="70"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="20"/>
       <c r="E10" s="20"/>
       <c r="F10" s="21"/>
@@ -12606,7 +12589,7 @@
     <col min="24" max="24" width="13.83203125" style="2" customWidth="1"/>
     <col min="25" max="25" width="13.83203125" style="3" customWidth="1"/>
     <col min="26" max="29" width="13.83203125" style="6" customWidth="1"/>
-    <col min="30" max="43" width="13.83203125" style="71" customWidth="1"/>
+    <col min="30" max="43" width="13.83203125" style="67" customWidth="1"/>
     <col min="44" max="46" width="13.83203125" style="10" customWidth="1"/>
     <col min="47" max="47" width="13.83203125" style="8" customWidth="1"/>
     <col min="48" max="49" width="13.83203125" style="10" customWidth="1"/>
@@ -12614,207 +12597,207 @@
     <col min="52" max="77" width="10.83203125" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:77" s="73" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="73" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="73" t="s">
+    <row r="1" spans="1:77" s="69" customFormat="1" ht="41" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="69" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="69" t="s">
         <v>50</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="69" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="74" t="s">
+      <c r="G1" s="70" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="73" t="s">
+      <c r="I1" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="73" t="s">
+      <c r="J1" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="K1" s="74" t="s">
+      <c r="K1" s="70" t="s">
         <v>42</v>
       </c>
-      <c r="L1" s="73" t="s">
+      <c r="L1" s="69" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="74" t="s">
+      <c r="M1" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="N1" s="73" t="s">
+      <c r="N1" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="O1" s="73" t="s">
+      <c r="O1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="P1" s="73" t="s">
+      <c r="P1" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="Q1" s="74" t="s">
+      <c r="Q1" s="70" t="s">
         <v>43</v>
       </c>
-      <c r="R1" s="73" t="s">
+      <c r="R1" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="73" t="s">
+      <c r="S1" s="69" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="73" t="s">
+      <c r="T1" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="74" t="s">
+      <c r="U1" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="V1" s="73" t="s">
+      <c r="V1" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="73" t="s">
+      <c r="W1" s="69" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="74" t="s">
+      <c r="X1" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="Y1" s="73" t="s">
+      <c r="Y1" s="69" t="s">
         <v>17</v>
       </c>
-      <c r="Z1" s="74" t="s">
+      <c r="Z1" s="70" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="73" t="s">
+      <c r="AA1" s="69" t="s">
         <v>18</v>
       </c>
-      <c r="AB1" s="73" t="s">
+      <c r="AB1" s="69" t="s">
         <v>8</v>
       </c>
-      <c r="AC1" s="73" t="s">
+      <c r="AC1" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="AD1" s="73" t="s">
+      <c r="AD1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="AE1" s="75" t="s">
+      <c r="AE1" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="AF1" s="73" t="s">
+      <c r="AF1" s="69" t="s">
         <v>23</v>
       </c>
-      <c r="AG1" s="73" t="s">
+      <c r="AG1" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="AH1" s="73" t="s">
+      <c r="AH1" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="AI1" s="73" t="s">
+      <c r="AI1" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="AJ1" s="73" t="s">
+      <c r="AJ1" s="69" t="s">
         <v>27</v>
       </c>
-      <c r="AK1" s="73" t="s">
+      <c r="AK1" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="AL1" s="73" t="s">
+      <c r="AL1" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="73" t="s">
+      <c r="AM1" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="AN1" s="73" t="s">
+      <c r="AN1" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="AO1" s="73" t="s">
+      <c r="AO1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="AP1" s="73" t="s">
+      <c r="AP1" s="69" t="s">
         <v>33</v>
       </c>
-      <c r="AQ1" s="73" t="s">
+      <c r="AQ1" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="AR1" s="73" t="s">
+      <c r="AR1" s="69" t="s">
         <v>34</v>
       </c>
-      <c r="AS1" s="73" t="s">
+      <c r="AS1" s="69" t="s">
         <v>19</v>
       </c>
-      <c r="AT1" s="73" t="s">
+      <c r="AT1" s="69" t="s">
         <v>35</v>
       </c>
-      <c r="AU1" s="73" t="s">
+      <c r="AU1" s="69" t="s">
         <v>36</v>
       </c>
-      <c r="AV1" s="73" t="s">
+      <c r="AV1" s="69" t="s">
         <v>37</v>
       </c>
-      <c r="AW1" s="73" t="s">
+      <c r="AW1" s="69" t="s">
         <v>38</v>
       </c>
-      <c r="AX1" s="73" t="s">
+      <c r="AX1" s="69" t="s">
         <v>39</v>
       </c>
-      <c r="AY1" s="73" t="s">
+      <c r="AY1" s="69" t="s">
         <v>40</v>
       </c>
-      <c r="AZ1" s="76"/>
-      <c r="BA1" s="76"/>
-      <c r="BB1" s="76"/>
-      <c r="BC1" s="76"/>
-      <c r="BD1" s="76"/>
-      <c r="BE1" s="76"/>
-      <c r="BF1" s="76"/>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="76"/>
-      <c r="BI1" s="76"/>
-      <c r="BJ1" s="76"/>
-      <c r="BK1" s="76"/>
-      <c r="BL1" s="76"/>
-      <c r="BM1" s="76"/>
-      <c r="BN1" s="76"/>
-      <c r="BO1" s="76"/>
-      <c r="BP1" s="76"/>
-      <c r="BQ1" s="76"/>
-      <c r="BR1" s="76"/>
-      <c r="BS1" s="76"/>
-      <c r="BT1" s="76"/>
-      <c r="BU1" s="76"/>
-      <c r="BV1" s="76"/>
-      <c r="BW1" s="76"/>
-      <c r="BX1" s="76"/>
-      <c r="BY1" s="76"/>
-    </row>
-    <row r="2" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="49" t="s">
-        <v>145</v>
-      </c>
-      <c r="B2" s="50">
+      <c r="AZ1" s="72"/>
+      <c r="BA1" s="72"/>
+      <c r="BB1" s="72"/>
+      <c r="BC1" s="72"/>
+      <c r="BD1" s="72"/>
+      <c r="BE1" s="72"/>
+      <c r="BF1" s="72"/>
+      <c r="BG1" s="72"/>
+      <c r="BH1" s="72"/>
+      <c r="BI1" s="72"/>
+      <c r="BJ1" s="72"/>
+      <c r="BK1" s="72"/>
+      <c r="BL1" s="72"/>
+      <c r="BM1" s="72"/>
+      <c r="BN1" s="72"/>
+      <c r="BO1" s="72"/>
+      <c r="BP1" s="72"/>
+      <c r="BQ1" s="72"/>
+      <c r="BR1" s="72"/>
+      <c r="BS1" s="72"/>
+      <c r="BT1" s="72"/>
+      <c r="BU1" s="72"/>
+      <c r="BV1" s="72"/>
+      <c r="BW1" s="72"/>
+      <c r="BX1" s="72"/>
+      <c r="BY1" s="72"/>
+    </row>
+    <row r="2" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="B2" s="46">
         <v>42.343719999999998</v>
       </c>
-      <c r="C2" s="51">
+      <c r="C2" s="47">
         <v>13.4503</v>
       </c>
-      <c r="D2" s="52">
+      <c r="D2" s="48">
         <v>644</v>
       </c>
       <c r="E2" s="10">
         <v>0</v>
       </c>
-      <c r="F2" s="53">
+      <c r="F2" s="49">
         <v>1338527.5950839354</v>
       </c>
-      <c r="G2" s="53">
+      <c r="G2" s="49">
         <v>45561.905833558922</v>
       </c>
       <c r="H2" s="10">
@@ -12823,30 +12806,30 @@
       <c r="I2" s="10">
         <v>2</v>
       </c>
-      <c r="J2" s="54">
+      <c r="J2" s="50">
         <v>150000</v>
       </c>
       <c r="K2" s="9">
         <f>J2*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L2" s="55">
+      <c r="L2" s="51">
         <v>60.141385601410576</v>
       </c>
-      <c r="M2" s="56">
+      <c r="M2" s="52">
         <f>0.1*L2</f>
         <v>6.014138560141058</v>
       </c>
-      <c r="N2" s="57">
+      <c r="N2" s="53">
         <v>0</v>
       </c>
       <c r="O2" s="10">
         <v>3.0874999999999989E-2</v>
       </c>
-      <c r="P2" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q2" s="58">
+      <c r="P2" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="54">
         <v>0</v>
       </c>
       <c r="R2" s="10">
@@ -12855,7 +12838,7 @@
       <c r="S2" s="10">
         <v>0.38950000000000023</v>
       </c>
-      <c r="T2" s="77">
+      <c r="T2" s="73">
         <f>392246.338278751*1.3994*0.0001</f>
         <v>54.890952578728417</v>
       </c>
@@ -12863,25 +12846,25 @@
         <f>0.1*T2</f>
         <v>5.489095257872842</v>
       </c>
-      <c r="V2" s="60">
-        <v>0</v>
-      </c>
-      <c r="W2" s="60">
-        <v>0</v>
-      </c>
-      <c r="X2" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y2" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z2" s="60">
+      <c r="V2" s="56">
+        <v>0</v>
+      </c>
+      <c r="W2" s="56">
+        <v>0</v>
+      </c>
+      <c r="X2" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="56">
         <v>0</v>
       </c>
       <c r="AA2" s="10">
         <v>3.3749999999999968E-2</v>
       </c>
-      <c r="AB2" s="60">
+      <c r="AB2" s="56">
         <v>0</v>
       </c>
       <c r="AC2" s="10">
@@ -12890,13 +12873,13 @@
       <c r="AD2" s="10">
         <v>43.849999999999966</v>
       </c>
-      <c r="AE2" s="60">
+      <c r="AE2" s="56">
         <v>0</v>
       </c>
       <c r="AF2" s="10">
         <v>3.0874999999999989E-2</v>
       </c>
-      <c r="AG2" s="60">
+      <c r="AG2" s="56">
         <v>0</v>
       </c>
       <c r="AH2" s="10">
@@ -12908,13 +12891,13 @@
       <c r="AJ2" s="10">
         <v>54.521458333333335</v>
       </c>
-      <c r="AK2" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="60">
+      <c r="AK2" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="56">
         <v>0</v>
       </c>
       <c r="AN2" s="10">
@@ -12929,7 +12912,7 @@
       <c r="AQ2" s="10">
         <v>1.5000000000000012E-2</v>
       </c>
-      <c r="AR2" s="60">
+      <c r="AR2" s="56">
         <v>0</v>
       </c>
       <c r="AS2" s="10">
@@ -12980,26 +12963,26 @@
       <c r="BX2" s="23"/>
       <c r="BY2" s="23"/>
     </row>
-    <row r="3" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="49" t="s">
-        <v>146</v>
-      </c>
-      <c r="B3" s="50">
+    <row r="3" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="45" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="46">
         <v>42.343440000000001</v>
       </c>
-      <c r="C3" s="51">
+      <c r="C3" s="47">
         <v>13.448880000000001</v>
       </c>
-      <c r="D3" s="52">
+      <c r="D3" s="48">
         <v>710</v>
       </c>
       <c r="E3" s="10">
         <v>0</v>
       </c>
-      <c r="F3" s="53">
+      <c r="F3" s="49">
         <v>2140347.5677868826</v>
       </c>
-      <c r="G3" s="53">
+      <c r="G3" s="49">
         <v>74021.305900001666</v>
       </c>
       <c r="H3" s="10">
@@ -13008,30 +12991,30 @@
       <c r="I3" s="10">
         <v>8</v>
       </c>
-      <c r="J3" s="54">
+      <c r="J3" s="50">
         <v>150000</v>
       </c>
       <c r="K3" s="9">
         <f t="shared" ref="K3:K4" si="0">J3*0.1</f>
         <v>15000</v>
       </c>
-      <c r="L3" s="55">
+      <c r="L3" s="51">
         <v>69.25349620861158</v>
       </c>
-      <c r="M3" s="56">
+      <c r="M3" s="52">
         <f>0.1*L3</f>
         <v>6.9253496208611587</v>
       </c>
-      <c r="N3" s="57">
+      <c r="N3" s="53">
         <v>0</v>
       </c>
       <c r="O3" s="10">
         <v>3.0874999999999989E-2</v>
       </c>
-      <c r="P3" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="58">
+      <c r="P3" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="54">
         <v>0</v>
       </c>
       <c r="R3" s="10">
@@ -13040,7 +13023,7 @@
       <c r="S3" s="10">
         <v>0.38950000000000023</v>
       </c>
-      <c r="T3" s="77">
+      <c r="T3" s="73">
         <f>399563.141036486*1.3994*0.0001</f>
         <v>55.914865956645855</v>
       </c>
@@ -13048,25 +13031,25 @@
         <f>0.1*T3</f>
         <v>5.5914865956645858</v>
       </c>
-      <c r="V3" s="60">
-        <v>0</v>
-      </c>
-      <c r="W3" s="60">
-        <v>0</v>
-      </c>
-      <c r="X3" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="60">
+      <c r="V3" s="56">
+        <v>0</v>
+      </c>
+      <c r="W3" s="56">
+        <v>0</v>
+      </c>
+      <c r="X3" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="56">
         <v>0</v>
       </c>
       <c r="AA3" s="10">
         <v>3.3749999999999968E-2</v>
       </c>
-      <c r="AB3" s="60">
+      <c r="AB3" s="56">
         <v>0</v>
       </c>
       <c r="AC3" s="10">
@@ -13075,13 +13058,13 @@
       <c r="AD3" s="10">
         <v>43.849999999999966</v>
       </c>
-      <c r="AE3" s="60">
+      <c r="AE3" s="56">
         <v>0</v>
       </c>
       <c r="AF3" s="10">
         <v>3.0874999999999989E-2</v>
       </c>
-      <c r="AG3" s="60">
+      <c r="AG3" s="56">
         <v>0</v>
       </c>
       <c r="AH3" s="10">
@@ -13093,13 +13076,13 @@
       <c r="AJ3" s="10">
         <v>54.521458333333335</v>
       </c>
-      <c r="AK3" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="60">
+      <c r="AK3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL3" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="56">
         <v>0</v>
       </c>
       <c r="AN3" s="10">
@@ -13114,7 +13097,7 @@
       <c r="AQ3" s="10">
         <v>1.5000000000000012E-2</v>
       </c>
-      <c r="AR3" s="60">
+      <c r="AR3" s="56">
         <v>0</v>
       </c>
       <c r="AS3" s="10">
@@ -13165,26 +13148,26 @@
       <c r="BX3" s="23"/>
       <c r="BY3" s="23"/>
     </row>
-    <row r="4" spans="1:77" s="49" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="49" t="s">
-        <v>147</v>
-      </c>
-      <c r="B4" s="50">
+    <row r="4" spans="1:77" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="45" t="s">
+        <v>144</v>
+      </c>
+      <c r="B4" s="46">
         <v>42.342979999999997</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="47">
         <v>13.44941</v>
       </c>
-      <c r="D4" s="61">
+      <c r="D4" s="57">
         <v>721</v>
       </c>
       <c r="E4" s="10">
         <v>0</v>
       </c>
-      <c r="F4" s="53">
+      <c r="F4" s="49">
         <v>2549765.5339940144</v>
       </c>
-      <c r="G4" s="53">
+      <c r="G4" s="49">
         <v>93875.094622778604</v>
       </c>
       <c r="H4" s="10">
@@ -13193,30 +13176,30 @@
       <c r="I4" s="10">
         <v>2.5</v>
       </c>
-      <c r="J4" s="54">
+      <c r="J4" s="50">
         <v>150000</v>
       </c>
       <c r="K4" s="9">
         <f t="shared" si="0"/>
         <v>15000</v>
       </c>
-      <c r="L4" s="55">
+      <c r="L4" s="51">
         <v>91.076858190610054</v>
       </c>
-      <c r="M4" s="56">
+      <c r="M4" s="52">
         <f>0.1*L4</f>
         <v>9.1076858190610057</v>
       </c>
-      <c r="N4" s="57">
+      <c r="N4" s="53">
         <v>0</v>
       </c>
       <c r="O4" s="10">
         <v>3.0874999999999989E-2</v>
       </c>
-      <c r="P4" s="58">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="58">
+      <c r="P4" s="54">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="54">
         <v>0</v>
       </c>
       <c r="R4" s="10">
@@ -13225,7 +13208,7 @@
       <c r="S4" s="10">
         <v>0.38950000000000023</v>
       </c>
-      <c r="T4" s="77">
+      <c r="T4" s="73">
         <f>358345.171827215*1.3994*0.0001</f>
         <v>50.146823345500472</v>
       </c>
@@ -13233,25 +13216,25 @@
         <f>0.1*T4</f>
         <v>5.0146823345500477</v>
       </c>
-      <c r="V4" s="60">
-        <v>0</v>
-      </c>
-      <c r="W4" s="60">
-        <v>0</v>
-      </c>
-      <c r="X4" s="60">
-        <v>0</v>
-      </c>
-      <c r="Y4" s="60">
-        <v>0</v>
-      </c>
-      <c r="Z4" s="60">
+      <c r="V4" s="56">
+        <v>0</v>
+      </c>
+      <c r="W4" s="56">
+        <v>0</v>
+      </c>
+      <c r="X4" s="56">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="56">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="56">
         <v>0</v>
       </c>
       <c r="AA4" s="10">
         <v>3.3749999999999968E-2</v>
       </c>
-      <c r="AB4" s="60">
+      <c r="AB4" s="56">
         <v>0</v>
       </c>
       <c r="AC4" s="10">
@@ -13260,13 +13243,13 @@
       <c r="AD4" s="10">
         <v>43.849999999999966</v>
       </c>
-      <c r="AE4" s="60">
+      <c r="AE4" s="56">
         <v>0</v>
       </c>
       <c r="AF4" s="10">
         <v>3.0874999999999989E-2</v>
       </c>
-      <c r="AG4" s="60">
+      <c r="AG4" s="56">
         <v>0</v>
       </c>
       <c r="AH4" s="10">
@@ -13278,13 +13261,13 @@
       <c r="AJ4" s="10">
         <v>54.521458333333335</v>
       </c>
-      <c r="AK4" s="60">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="60">
-        <v>0</v>
-      </c>
-      <c r="AM4" s="60">
+      <c r="AK4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AL4" s="56">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="56">
         <v>0</v>
       </c>
       <c r="AN4" s="10">
@@ -13299,7 +13282,7 @@
       <c r="AQ4" s="10">
         <v>1.5000000000000012E-2</v>
       </c>
-      <c r="AR4" s="60">
+      <c r="AR4" s="56">
         <v>0</v>
       </c>
       <c r="AS4" s="10">

</xml_diff>